<commit_message>
prepare menu & role & user
</commit_message>
<xml_diff>
--- a/数据表设计.xlsx
+++ b/数据表设计.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="目录" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="364">
   <si>
     <t xml:space="preserve">#数据字典</t>
   </si>
@@ -224,15 +224,18 @@
     <t xml:space="preserve">机构名称</t>
   </si>
   <si>
-    <t xml:space="preserve">number</t>
-  </si>
-  <si>
     <t xml:space="preserve">admin_code</t>
   </si>
   <si>
     <t xml:space="preserve">账户名称</t>
   </si>
   <si>
+    <t xml:space="preserve">role_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">角色编码</t>
+  </si>
+  <si>
     <t xml:space="preserve">initial_password</t>
   </si>
   <si>
@@ -290,7 +293,7 @@
     <t xml:space="preserve">teacher_count</t>
   </si>
   <si>
-    <t xml:space="preserve">任课教师总数(人)</t>
+    <t xml:space="preserve">任课教师总数（人）</t>
   </si>
   <si>
     <t xml:space="preserve">integer</t>
@@ -299,31 +302,31 @@
     <t xml:space="preserve">student_count</t>
   </si>
   <si>
-    <t xml:space="preserve">学生总数(人)</t>
+    <t xml:space="preserve">学生总数（人）</t>
   </si>
   <si>
     <t xml:space="preserve">room_count</t>
   </si>
   <si>
-    <t xml:space="preserve">教室（含功能室）总数(间)</t>
+    <t xml:space="preserve">教室（含功能室）总数（间）</t>
   </si>
   <si>
     <t xml:space="preserve">classroom_count</t>
   </si>
   <si>
-    <t xml:space="preserve">班级教室总数(间)</t>
+    <t xml:space="preserve">班级教室总数（间）</t>
   </si>
   <si>
     <t xml:space="preserve">student_desk_count</t>
   </si>
   <si>
-    <t xml:space="preserve">学生课桌椅可用数(套)</t>
+    <t xml:space="preserve">学生课桌椅可用数（套）</t>
   </si>
   <si>
     <t xml:space="preserve">connected_room_count</t>
   </si>
   <si>
-    <t xml:space="preserve">已入网教室数(间)</t>
+    <t xml:space="preserve">已入网教室数（间）</t>
   </si>
   <si>
     <t xml:space="preserve">has_a_central_server_room</t>
@@ -416,32 +419,7 @@
     <t xml:space="preserve">宣传平台责任人</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">equipment_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">funds</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_this_year</t>
-    </r>
+    <t xml:space="preserve">equipment_funds_this_year</t>
   </si>
   <si>
     <t xml:space="preserve">本年设备维护投入资金（万元）</t>
@@ -784,17 +762,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">cabinet</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">_num</t>
+      <t xml:space="preserve">cabinet_num</t>
     </r>
   </si>
   <si>
@@ -1666,7 +1636,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK SC"/>
@@ -1706,16 +1676,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Noto Sans CJK SC"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1906,11 +1866,11 @@
   </sheetPr>
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.04"/>
   </cols>
@@ -2005,7 +1965,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.76"/>
@@ -2020,7 +1980,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,7 +2011,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>46</v>
@@ -2066,10 +2026,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>46</v>
@@ -2084,13 +2044,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
@@ -2100,31 +2060,31 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>8.2</v>
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="11"/>
@@ -2134,13 +2094,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="11"/>
@@ -2150,13 +2110,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>8.2</v>
@@ -2168,13 +2128,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="11"/>
@@ -2184,13 +2144,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>8.2</v>
@@ -2202,29 +2162,29 @@
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="n">
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="11"/>
@@ -2234,13 +2194,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="11"/>
@@ -2250,13 +2210,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E16" s="3" t="n">
         <v>8.2</v>
@@ -2268,13 +2228,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="11"/>
@@ -2284,13 +2244,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E18" s="3" t="n">
         <v>8.2</v>
@@ -2302,29 +2262,29 @@
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="n">
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="14"/>
@@ -2334,13 +2294,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="14"/>
@@ -2350,13 +2310,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>8.2</v>
@@ -2368,13 +2328,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="14"/>
@@ -2384,10 +2344,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>46</v>
@@ -2593,7 +2553,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.85"/>
@@ -2608,7 +2568,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,7 +2599,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>46</v>
@@ -2654,10 +2614,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>46</v>
@@ -2672,13 +2632,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
@@ -2688,13 +2648,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>8.2</v>
@@ -2706,13 +2666,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="11"/>
@@ -2722,13 +2682,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="11"/>
@@ -2738,13 +2698,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>8.2</v>
@@ -2756,13 +2716,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="11"/>
@@ -2772,13 +2732,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>8.2</v>
@@ -2790,13 +2750,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="11"/>
@@ -2806,13 +2766,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="11"/>
@@ -2822,13 +2782,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E15" s="3" t="n">
         <v>8.2</v>
@@ -2840,13 +2800,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="11"/>
@@ -2856,13 +2816,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E17" s="3" t="n">
         <v>8.2</v>
@@ -2874,13 +2834,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="11"/>
@@ -2890,13 +2850,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="11"/>
@@ -2906,13 +2866,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>8.2</v>
@@ -2924,13 +2884,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="14"/>
@@ -2940,10 +2900,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>46</v>
@@ -2958,13 +2918,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="14"/>
@@ -2974,13 +2934,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>8.2</v>
@@ -2992,10 +2952,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>46</v>
@@ -3009,13 +2969,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E26" s="2"/>
     </row>
@@ -3024,13 +2984,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E27" s="2" t="n">
         <v>8.2</v>
@@ -3209,7 +3169,7 @@
       <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.94"/>
@@ -3224,7 +3184,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3255,7 +3215,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>46</v>
@@ -3270,10 +3230,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>46</v>
@@ -3288,13 +3248,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
@@ -3304,13 +3264,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="11"/>
@@ -3320,13 +3280,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="11"/>
@@ -3336,13 +3296,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="11"/>
@@ -3352,13 +3312,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="11"/>
@@ -3368,13 +3328,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="11"/>
@@ -3384,13 +3344,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="11"/>
@@ -3400,13 +3360,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="11"/>
@@ -3416,13 +3376,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="11"/>
@@ -3432,13 +3392,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="11"/>
@@ -3448,13 +3408,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="11"/>
@@ -3464,13 +3424,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="11"/>
@@ -3480,10 +3440,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>46</v>
@@ -3500,10 +3460,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>46</v>
@@ -3520,13 +3480,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="14"/>
@@ -3536,13 +3496,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="14"/>
@@ -3552,13 +3512,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="14"/>
@@ -3568,13 +3528,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="14"/>
@@ -3781,7 +3741,7 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="22.92"/>
@@ -4694,13 +4654,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.66"/>
@@ -4784,7 +4744,7 @@
         <v>20</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E6" s="11" t="n">
         <v>2</v>
@@ -4798,10 +4758,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>46</v>
@@ -4816,16 +4776,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="11" t="n">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F8" s="11"/>
     </row>
@@ -4834,49 +4794,60 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>30</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>46</v>
       </c>
       <c r="E10" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="11" t="n">
+        <v>30</v>
+      </c>
       <c r="F11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -4884,7 +4855,6 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -4936,6 +4906,14 @@
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4956,13 +4934,13 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.56"/>
@@ -4973,7 +4951,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5001,10 +4979,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>46</v>
@@ -5019,10 +4997,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>46</v>
@@ -5037,10 +5015,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>46</v>
@@ -5057,13 +5035,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -5182,10 +5160,10 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.66"/>
@@ -5199,7 +5177,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5230,7 +5208,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>46</v>
@@ -5245,10 +5223,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>46</v>
@@ -5263,13 +5241,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -5279,13 +5257,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -5295,13 +5273,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -5311,13 +5289,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -5327,29 +5305,29 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -5359,10 +5337,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>46</v>
@@ -5379,13 +5357,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E13" s="11" t="n">
         <v>8.2</v>
@@ -5468,7 +5446,7 @@
       <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.07"/>
@@ -5483,7 +5461,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5514,7 +5492,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>46</v>
@@ -5529,10 +5507,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>46</v>
@@ -5547,10 +5525,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>46</v>
@@ -5565,10 +5543,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>46</v>
@@ -5583,10 +5561,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>46</v>
@@ -5601,10 +5579,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>46</v>
@@ -5619,10 +5597,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>46</v>
@@ -5637,10 +5615,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>46</v>
@@ -5655,10 +5633,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>46</v>
@@ -5673,10 +5651,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>46</v>
@@ -5691,10 +5669,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>46</v>
@@ -5709,10 +5687,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>46</v>
@@ -5727,10 +5705,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>46</v>
@@ -5745,10 +5723,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>46</v>
@@ -5763,13 +5741,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E18" s="11" t="n">
         <v>8.2</v>
@@ -5781,13 +5759,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
@@ -5797,13 +5775,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" s="11"/>
     </row>
@@ -5830,7 +5808,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74.19"/>
@@ -5845,7 +5823,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5876,7 +5854,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>46</v>
@@ -5891,10 +5869,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>46</v>
@@ -5909,13 +5887,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -5925,13 +5903,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>8.2</v>
@@ -5943,13 +5921,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -5959,13 +5937,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -5975,13 +5953,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>8.2</v>
@@ -5993,13 +5971,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -6009,13 +5987,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -6025,13 +6003,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -6041,13 +6019,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E14" s="3" t="n">
         <v>8.2</v>
@@ -6059,13 +6037,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -6075,13 +6053,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -6091,13 +6069,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E17" s="3" t="n">
         <v>8.2</v>
@@ -6109,13 +6087,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -6125,13 +6103,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -6141,13 +6119,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
@@ -6157,13 +6135,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>8.2</v>
@@ -6175,13 +6153,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -6191,13 +6169,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -6207,13 +6185,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>8.2</v>
@@ -6225,13 +6203,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -6241,13 +6219,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -6257,13 +6235,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="3"/>
@@ -6273,13 +6251,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="3"/>
@@ -6289,13 +6267,13 @@
         <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E29" s="2"/>
     </row>
@@ -6457,7 +6435,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.71"/>
@@ -6472,7 +6450,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6503,7 +6481,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>46</v>
@@ -6518,10 +6496,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>46</v>
@@ -6536,13 +6514,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
@@ -6552,13 +6530,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>8.2</v>
@@ -6570,13 +6548,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>8.2</v>
@@ -6588,13 +6566,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="11"/>
@@ -6604,13 +6582,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="11"/>
@@ -6620,10 +6598,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>46</v>
@@ -6640,13 +6618,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>8.2</v>
@@ -6658,10 +6636,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>46</v>
@@ -6676,13 +6654,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="11"/>
@@ -6692,13 +6670,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E15" s="3" t="n">
         <v>8.2</v>
@@ -6710,10 +6688,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>46</v>
@@ -6728,13 +6706,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="11"/>
@@ -6744,13 +6722,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E18" s="3" t="n">
         <v>8.2</v>
@@ -6762,10 +6740,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>46</v>
@@ -6778,10 +6756,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>46</v>
@@ -7010,7 +6988,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.76"/>
@@ -7025,7 +7003,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7056,7 +7034,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>46</v>
@@ -7071,10 +7049,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>46</v>
@@ -7089,13 +7067,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="11"/>
@@ -7105,13 +7083,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>8.2</v>
@@ -7123,13 +7101,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>8.2</v>
@@ -7141,28 +7119,28 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>8.2</v>
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>46</v>
@@ -7174,15 +7152,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>46</v>
@@ -7194,15 +7172,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>46</v>
@@ -7219,13 +7197,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="11"/>
@@ -7235,13 +7213,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="11"/>
@@ -7251,13 +7229,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E15" s="3" t="n">
         <v>8.2</v>
@@ -7269,13 +7247,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E16" s="3" t="n">
         <v>8.2</v>
@@ -7287,13 +7265,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="11"/>
@@ -7303,13 +7281,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E18" s="3" t="n">
         <v>8.2</v>
@@ -7321,13 +7299,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="11"/>
@@ -7337,13 +7315,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -7352,13 +7330,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>8.2</v>
@@ -7369,13 +7347,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -7384,13 +7362,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" s="2"/>
     </row>
@@ -7399,13 +7377,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E24" s="2" t="n">
         <v>8.2</v>
@@ -7416,13 +7394,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -7431,13 +7409,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E26" s="2"/>
     </row>

</xml_diff>